<commit_message>
Fixed oscillator caps, began changing resistors to more common values
</commit_message>
<xml_diff>
--- a/Part List.xlsx
+++ b/Part List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krotain\Documents\git\493\ece_492-3_topic_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2E2B1F-60A9-4C60-9374-F8324AF25940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9753571-44CA-4775-897C-229F1B427246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2175" windowWidth="29040" windowHeight="16440" xr2:uid="{DD9C814F-33BB-46B4-954A-62ACB4677A0F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="125">
   <si>
     <t>Part</t>
   </si>
@@ -149,9 +149,6 @@
     <t>10nf</t>
   </si>
   <si>
-    <t>220p</t>
-  </si>
-  <si>
     <t>CL21B223KBANFNC</t>
   </si>
   <si>
@@ -246,6 +243,174 @@
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/STMicroelectronics/L6902D?qs=Yc96klrMi5L2iIsse6YmdQ%3D%3D</t>
+  </si>
+  <si>
+    <t>INA180A1</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/INA180A1IDBVT/7219027?s=N4IgTCBcDaIJIDkCCBGAHABlXAIgIQDUAVEAXQF8g</t>
+  </si>
+  <si>
+    <t>PJA3404_R1_00001</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Panjit/PJA3404_R1_00001?qs=sPbYRqrBIVkiUO9ZInE3tw%3D%3D</t>
+  </si>
+  <si>
+    <t>TODO: SMD BJT</t>
+  </si>
+  <si>
+    <t>STM32L152RBT6A</t>
+  </si>
+  <si>
+    <t>LQFP-64</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/STMicroelectronics/STM32L152RBT6A?qs=DqCdCwOw4%2F646g2lv17dkw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/STMicroelectronics/STM32L100C6U6A?qs=9MuLHSklicr37J4PyR0bYg%3D%3D</t>
+  </si>
+  <si>
+    <t>UFQFPN-48</t>
+  </si>
+  <si>
+    <t>STM32L100C6U6A</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Vishay-Dale/XT9S20ANA8M?qs=oFi4%2FQsgZXYxL7wCZW5FzA%3D%3D</t>
+  </si>
+  <si>
+    <t>8MHz</t>
+  </si>
+  <si>
+    <t>Radial</t>
+  </si>
+  <si>
+    <t>HC-49/US</t>
+  </si>
+  <si>
+    <t>XT9S20ANA8M</t>
+  </si>
+  <si>
+    <t>20pf</t>
+  </si>
+  <si>
+    <t>220pf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL10C200JB8NNNC?qs=X6jEic%2FHinCxVzG4eDnU5g%3D%3D</t>
+  </si>
+  <si>
+    <t>CL10C200JB8NNNC</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>FS24-800-C2</t>
+  </si>
+  <si>
+    <t>Big</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Triad-Magnetics/FS24-800-C2?qs=b1anAsPanWysxDNUFWmxRA%3D%3D</t>
+  </si>
+  <si>
+    <t>RCH664NP-220K</t>
+  </si>
+  <si>
+    <t>22uh</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sumida-america-inc/RCH664NP-220K/3946785?s=N4IgTCBcDaIEoGEASA2FAWAcgBQLRjAAYBpEAXQF8g</t>
+  </si>
+  <si>
+    <t>KDV06FR180ET</t>
+  </si>
+  <si>
+    <t>180mOhm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Ohmite/KDV06FR180ET?qs=l4Gc20tDgJLuG9Oc1mkpPg%3D%3D</t>
+  </si>
+  <si>
+    <t>KDV06FR300ET</t>
+  </si>
+  <si>
+    <t>300mOhm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Ohmite/KDV06FR300ET?qs=l4Gc20tDgJIqinXnKONtAA%3D%3D</t>
+  </si>
+  <si>
+    <t>SDR03EZPF1002</t>
+  </si>
+  <si>
+    <t>10kOhm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/SDR03EZPF1002?qs=byeeYqUIh0Mlr2mre8duxQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF5101?qs=493kPxzlxfITg5G1s39ZCA%3D%3D</t>
+  </si>
+  <si>
+    <t>5.1kOhm</t>
+  </si>
+  <si>
+    <t>ESR03EZPF5101</t>
+  </si>
+  <si>
+    <t>ESR03EZPF4701</t>
+  </si>
+  <si>
+    <t>4.7kOhm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF4701?qs=493kPxzlxfL2NnaeJoZB2Q%3D%3D</t>
+  </si>
+  <si>
+    <t>1.2kOhm</t>
+  </si>
+  <si>
+    <t>ESR03EZPF1000</t>
+  </si>
+  <si>
+    <t>100Ohm</t>
+  </si>
+  <si>
+    <t>1kOhm</t>
+  </si>
+  <si>
+    <t>2kOhm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF1000?qs=493kPxzlxfJdLkJZpX4ByA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF2001?qs=493kPxzlxfIsacc9Eh0USA%3D%3D</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>ESR03EZPF2001</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF1001?qs=DyUWGjl%252BcVtUAf3p1rg3iQ%3D%3D</t>
+  </si>
+  <si>
+    <t>ESR03EZPF1001</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF1201?qs=493kPxzlxfIq0F4ql8poBA%3D%3D</t>
+  </si>
+  <si>
+    <t>ESR03EZPF1201</t>
   </si>
 </sst>
 </file>
@@ -623,16 +788,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABF4B5B-D5F0-478D-961E-5722ED7FBC19}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="6" max="7" width="9.85546875" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
     <col min="9" max="9" width="152.7109375" customWidth="1"/>
   </cols>
@@ -707,7 +872,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E20" si="0">D3*B3</f>
+        <f t="shared" ref="E3:E13" si="0">D3*B3</f>
         <v>0.63200000000000001</v>
       </c>
       <c r="F3" t="s">
@@ -875,7 +1040,7 @@
         <v>32</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>0.1</v>
@@ -885,7 +1050,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0.18</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="F9" t="s">
         <v>34</v>
@@ -897,12 +1062,12 @@
         <v>21</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -927,12 +1092,12 @@
         <v>21</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -957,12 +1122,12 @@
         <v>21</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -978,7 +1143,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G12" s="4">
         <v>0.1</v>
@@ -987,247 +1152,754 @@
         <v>21</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>0.46</v>
+        <v>0.1</v>
       </c>
       <c r="D13">
-        <v>0.14199999999999999</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0.28399999999999997</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" t="s">
-        <v>48</v>
+        <v>86</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.05</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14">
-        <v>0.84</v>
+        <v>0.46</v>
       </c>
       <c r="D14">
-        <v>0.28299999999999997</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>0.56599999999999995</v>
+        <f>D14*B14</f>
+        <v>0.28399999999999997</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15">
-        <v>0.38</v>
+        <v>0.84</v>
       </c>
       <c r="D15">
-        <v>0.11700000000000001</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>0.23400000000000001</v>
+        <f>D15*B15</f>
+        <v>0.56599999999999995</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16">
-        <v>0.21</v>
+        <v>0.38</v>
       </c>
       <c r="D16">
-        <v>0.114</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0.22800000000000001</v>
+        <f>D16*B16</f>
+        <v>0.23400000000000001</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16">
-        <v>1812</v>
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>52</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>5.6</v>
+        <v>1.05</v>
       </c>
       <c r="D17">
-        <v>3.1888000000000001</v>
+        <v>0.47839999999999999</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>3.1888000000000001</v>
+        <f>D17*B17</f>
+        <v>0.95679999999999998</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>0.76</v>
+        <v>0.37</v>
       </c>
       <c r="D18">
-        <v>0.32800000000000001</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0.65600000000000003</v>
+        <f>D18*B18</f>
+        <v>0.49199999999999999</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>6.41</v>
-      </c>
-      <c r="D19">
-        <v>3.41</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>6.82</v>
-      </c>
-      <c r="F19" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20">
+        <v>0.21</v>
+      </c>
+      <c r="D20">
+        <v>0.114</v>
+      </c>
+      <c r="E20">
+        <f>D20*B20</f>
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20">
+        <v>1812</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>5.6</v>
+      </c>
+      <c r="D21">
+        <v>3.1888000000000001</v>
+      </c>
+      <c r="E21">
+        <f>D21*B21</f>
+        <v>3.1888000000000001</v>
+      </c>
+      <c r="F21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>0.76</v>
+      </c>
+      <c r="D22">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="E22">
+        <f>D22*B22</f>
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="F22" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>6.41</v>
+      </c>
+      <c r="D23">
+        <v>3.41</v>
+      </c>
+      <c r="E23">
+        <f>D23*B23</f>
+        <v>6.82</v>
+      </c>
+      <c r="F23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
         <v>3.44</v>
       </c>
-      <c r="D20">
+      <c r="D24">
         <v>1.96</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
+      <c r="E24">
+        <f>D24*B24</f>
         <v>3.92</v>
       </c>
-      <c r="F20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="F24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>69</v>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>8.06</v>
+      </c>
+      <c r="D25">
+        <v>4.51</v>
+      </c>
+      <c r="E25">
+        <f>D25*B25</f>
+        <v>4.51</v>
+      </c>
+      <c r="F25" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>5.57</v>
+      </c>
+      <c r="D26">
+        <v>2.95</v>
+      </c>
+      <c r="E26">
+        <f>D26*B26</f>
+        <v>2.95</v>
+      </c>
+      <c r="F26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" t="s">
+        <v>79</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>0.44</v>
+      </c>
+      <c r="D27">
+        <v>0.31</v>
+      </c>
+      <c r="E27">
+        <f>D27*B27</f>
+        <v>0.62</v>
+      </c>
+      <c r="F27" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" t="s">
+        <v>84</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>16.5</v>
+      </c>
+      <c r="D28">
+        <v>9.82</v>
+      </c>
+      <c r="E28">
+        <f>D28*B28</f>
+        <v>9.82</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" t="s">
+        <v>92</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>0.94</v>
+      </c>
+      <c r="D29">
+        <v>0.43</v>
+      </c>
+      <c r="E29">
+        <f>D29*B29</f>
+        <v>2.58</v>
+      </c>
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>83</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>0.26</v>
+      </c>
+      <c r="D30">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E30">
+        <f>D30*B30</f>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>0.26</v>
+      </c>
+      <c r="D31">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="E31">
+        <f>D31*B31</f>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D32">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E32">
+        <f>D32*B32</f>
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D33">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E33">
+        <f>D33*B33</f>
+        <v>0.126</v>
+      </c>
+      <c r="F33" t="s">
+        <v>107</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D34">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E34">
+        <f>D34*B34</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>124</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D35">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E35">
+        <f>D35*B35</f>
+        <v>0.126</v>
+      </c>
+      <c r="F35" t="s">
+        <v>112</v>
+      </c>
+      <c r="G35" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D36">
+        <v>2.4E-2</v>
+      </c>
+      <c r="E36">
+        <f>D36*B36</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37">
+        <v>0.15</v>
+      </c>
+      <c r="D37">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>115</v>
+      </c>
+      <c r="G37" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D38">
+        <v>2.4E-2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>116</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1244,16 +1916,33 @@
     <hyperlink ref="I9" r:id="rId9" xr:uid="{5910EA08-9E19-4F72-9ADB-C3DC943A9880}"/>
     <hyperlink ref="I11" r:id="rId10" xr:uid="{336ACA25-DF51-493A-B97B-7384AE7BF67B}"/>
     <hyperlink ref="I12" r:id="rId11" xr:uid="{63A18238-7A07-49F3-A985-3D844C29C2CB}"/>
-    <hyperlink ref="I13" r:id="rId12" xr:uid="{2E91CEEF-D030-42BD-8B62-5BA748F4BFB7}"/>
-    <hyperlink ref="I14" r:id="rId13" xr:uid="{C09D32E1-5978-432C-95AA-B215B3A36ED3}"/>
-    <hyperlink ref="I15" r:id="rId14" xr:uid="{710A736C-147F-44A6-980D-F8ED04995C2A}"/>
-    <hyperlink ref="I16" r:id="rId15" xr:uid="{92C36C49-CEB7-4A72-B877-A11899E89BE2}"/>
-    <hyperlink ref="I18" r:id="rId16" xr:uid="{4EB0278A-4B3D-430B-A61C-80C7370DCF6F}"/>
-    <hyperlink ref="I17" r:id="rId17" xr:uid="{BF6DE5DC-89C2-4BD8-AE62-76723EEEDE83}"/>
-    <hyperlink ref="I19" r:id="rId18" xr:uid="{486F8D7D-0B15-47C5-9D97-1AA471F91B5D}"/>
-    <hyperlink ref="I20" r:id="rId19" xr:uid="{D136844E-AA85-4E69-B0DA-01D3AFD45890}"/>
+    <hyperlink ref="I14" r:id="rId12" xr:uid="{2E91CEEF-D030-42BD-8B62-5BA748F4BFB7}"/>
+    <hyperlink ref="I15" r:id="rId13" xr:uid="{C09D32E1-5978-432C-95AA-B215B3A36ED3}"/>
+    <hyperlink ref="I16" r:id="rId14" xr:uid="{710A736C-147F-44A6-980D-F8ED04995C2A}"/>
+    <hyperlink ref="I20" r:id="rId15" xr:uid="{92C36C49-CEB7-4A72-B877-A11899E89BE2}"/>
+    <hyperlink ref="I22" r:id="rId16" xr:uid="{4EB0278A-4B3D-430B-A61C-80C7370DCF6F}"/>
+    <hyperlink ref="I21" r:id="rId17" xr:uid="{BF6DE5DC-89C2-4BD8-AE62-76723EEEDE83}"/>
+    <hyperlink ref="I23" r:id="rId18" xr:uid="{486F8D7D-0B15-47C5-9D97-1AA471F91B5D}"/>
+    <hyperlink ref="I24" r:id="rId19" xr:uid="{D136844E-AA85-4E69-B0DA-01D3AFD45890}"/>
+    <hyperlink ref="I17" r:id="rId20" xr:uid="{5938C70C-9994-491E-8C8E-714909A51FC5}"/>
+    <hyperlink ref="I18" r:id="rId21" xr:uid="{09D08152-5192-4B18-A262-9992FC42F93A}"/>
+    <hyperlink ref="I25" r:id="rId22" xr:uid="{8C33B197-A161-4837-82ED-5B68E46D5DF7}"/>
+    <hyperlink ref="I26" r:id="rId23" xr:uid="{F3FBB0A4-3902-4DAF-A37B-76F301E09156}"/>
+    <hyperlink ref="I27" r:id="rId24" xr:uid="{AFE4F09A-555F-42AA-B131-38F6ED42FEB3}"/>
+    <hyperlink ref="I28" r:id="rId25" xr:uid="{023AC9E4-D4A9-4F9F-A849-E84F4EC49E5C}"/>
+    <hyperlink ref="I29" r:id="rId26" xr:uid="{82910215-DA44-4972-8AD3-BC2EF13D8673}"/>
+    <hyperlink ref="I30" r:id="rId27" xr:uid="{09D3FEA4-5ABC-4407-99EB-DFD5FEF8F848}"/>
+    <hyperlink ref="I31" r:id="rId28" xr:uid="{9FC6225D-D32E-4A1B-BCB1-3C48474CD21B}"/>
+    <hyperlink ref="I13" r:id="rId29" xr:uid="{BDD89C76-645C-4FB0-A077-0F3054C86712}"/>
+    <hyperlink ref="I32" r:id="rId30" xr:uid="{B2D7D052-A1D1-415D-B230-8957BB283201}"/>
+    <hyperlink ref="I33" r:id="rId31" xr:uid="{250A83A0-C654-4E28-9F2F-BD3ADC2DD1C3}"/>
+    <hyperlink ref="I34" r:id="rId32" xr:uid="{D3DFAAE9-3735-43A8-8793-71C985FB4FBD}"/>
+    <hyperlink ref="I35" r:id="rId33" xr:uid="{19ECA42A-A782-4EA0-882E-A4E617FFCBC6}"/>
+    <hyperlink ref="I36" r:id="rId34" xr:uid="{B9D01495-AA86-4548-AD27-CA6C7A678A28}"/>
+    <hyperlink ref="I38" r:id="rId35" xr:uid="{8B3B765E-E142-444F-8ED5-BEFBF459EAEB}"/>
+    <hyperlink ref="I37" r:id="rId36" xr:uid="{76DF0F02-5C82-45C2-9680-F9E4B8763809}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed capacitors to x7r
</commit_message>
<xml_diff>
--- a/Part List.xlsx
+++ b/Part List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krotain\Documents\git\493\ece_492-3_topic_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DA71EB-0137-460D-ABE5-86ABFD0F2C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2444021C-7ED2-48FF-BC6B-5CD504849F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2175" windowWidth="29040" windowHeight="16440" xr2:uid="{DD9C814F-33BB-46B4-954A-62ACB4677A0F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="156">
   <si>
     <t>Quantity</t>
   </si>
@@ -86,39 +86,21 @@
     <t>CL21A226MAYNNNE</t>
   </si>
   <si>
-    <t>CL21A106KAYNNNG</t>
-  </si>
-  <si>
     <t>10uf</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL21A106KAYNNNG?qs=sGAEpiMZZMsh%252B1woXyUXj%252BV5GOLijFH81pibuAyqgo4%3D</t>
-  </si>
-  <si>
     <t>0805</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL21A475KAQNNNE?qs=sGAEpiMZZMsh%252B1woXyUXj%252BV5GOLijFH8W2HE%252BxMgC1I%3D</t>
-  </si>
-  <si>
-    <t>CL21A475KAQNNNE</t>
-  </si>
-  <si>
     <t>4.7uf</t>
   </si>
   <si>
     <t>Tolerance</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL21A225KAFNNNE?qs=sGAEpiMZZMsh%252B1woXyUXjzRu9w46NtHrfF6fR2skA3I%3D</t>
-  </si>
-  <si>
     <t>2.2uf</t>
   </si>
   <si>
-    <t>CL21A225KAFNNNE</t>
-  </si>
-  <si>
     <t>1uf</t>
   </si>
   <si>
@@ -179,9 +161,6 @@
     <t>https://www.mouser.com/ProductDetail/onsemi/LP2950CDT-3.3RKG?qs=2OtswVQKCOGjJvIdedTxCw%3D%3D</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/texas-instruments/LM2672N-5-0-NOPB/363784</t>
-  </si>
-  <si>
     <t>LT3080EDD</t>
   </si>
   <si>
@@ -446,9 +425,6 @@
     <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL10B223KB85PNC?qs=349EhDEZ59qBh%2F6I4zsEtA%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL21A226MAYNNNE?qs=xZ%2FP%252Ba9zWqY%2FVvCfXjMhqg%3D%3D</t>
-  </si>
-  <si>
     <t>100uf</t>
   </si>
   <si>
@@ -501,6 +477,33 @@
   </si>
   <si>
     <t>552-*</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Diodes-Incorporated/AP63205WU-7?qs=u16ybLDytRZtkj8PzdWCOw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL21B225KAFNNNG?qs=yOVawPpwOwljM4cRphaUPg%3D%3D</t>
+  </si>
+  <si>
+    <t>CL21B225KAFNNNG</t>
+  </si>
+  <si>
+    <t>CL21B475KAFNNNE</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL21B475KAFNNNE?qs=fer0DVZjnG76MxvRzgkzzw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL31B106KAHNFNE?qs=xZ%2FP%252Ba9zWqbvZ%2FuLWvQDdQ%3D%3D</t>
+  </si>
+  <si>
+    <t>CL31B106KAHNFNE</t>
+  </si>
+  <si>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL32B226KAJNNNE?qs=349EhDEZ59oxUqah7LWaWw%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -880,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABF4B5B-D5F0-478D-961E-5722ED7FBC19}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +898,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -913,7 +916,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -922,7 +925,7 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -946,7 +949,7 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
@@ -956,7 +959,7 @@
       </c>
       <c r="J2">
         <f>SUM(E:E)</f>
-        <v>85.415760000000034</v>
+        <v>85.07976000000005</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -980,7 +983,7 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>14</v>
@@ -991,7 +994,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1007,21 +1010,21 @@
         <v>4.04</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G4" s="4">
         <v>0.2</v>
       </c>
       <c r="H4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1037,24 +1040,24 @@
         <v>0.874</v>
       </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G5" s="4">
         <v>0.2</v>
       </c>
       <c r="H5" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0.83</v>
@@ -1064,24 +1067,24 @@
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E16" si="1">D6*B6</f>
-        <v>2.1880000000000002</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G6" s="4">
         <v>0.2</v>
       </c>
       <c r="H6" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1097,16 +1100,16 @@
         <v>0.36</v>
       </c>
       <c r="F7" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G7" s="4">
         <v>0.2</v>
       </c>
       <c r="H7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1114,127 +1117,127 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>0.26</v>
+        <v>0.6</v>
       </c>
       <c r="D8">
-        <v>6.2E-2</v>
+        <v>0.17</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>0.496</v>
+        <v>2.04</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G8" s="4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>153</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9">
-        <v>0.18</v>
+        <v>0.23</v>
       </c>
       <c r="D9">
-        <v>3.6999999999999998E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>0.22199999999999998</v>
+        <v>0.28800000000000003</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="4">
         <v>0.1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>18</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>150</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10">
-        <v>0.1</v>
+        <v>0.43</v>
       </c>
       <c r="D10">
-        <v>0.02</v>
+        <v>0.126</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>0.252</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G10" s="4">
         <v>0.1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>20</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="D11">
-        <v>2.4E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>4.8000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G11" s="4">
         <v>0.1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>24</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>0.1</v>
@@ -1244,27 +1247,27 @@
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>0.121</v>
+        <v>9.8999999999999991E-2</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G12" s="4">
         <v>0.1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B13">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>0.1</v>
@@ -1274,24 +1277,24 @@
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>9.0999999999999998E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G13" s="4">
         <v>0.1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1307,21 +1310,21 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G14" s="4">
         <v>0.1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1337,24 +1340,24 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G15" s="4">
         <v>0.1</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>0.1</v>
@@ -1364,24 +1367,24 @@
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>4.3999999999999997E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G16" s="4">
         <v>0.05</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1397,21 +1400,21 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1427,21 +1430,21 @@
         <v>0.56599999999999995</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1457,21 +1460,21 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G19" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H19" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -1487,21 +1490,21 @@
         <v>0.95679999999999998</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H20" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1517,21 +1520,21 @@
         <v>0.49199999999999999</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H21" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -1547,21 +1550,21 @@
         <v>0.248</v>
       </c>
       <c r="F22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H22" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1577,21 +1580,21 @@
         <v>0.22800000000000001</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G23" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H23" s="2">
         <v>1812</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1607,21 +1610,21 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F24" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G24" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H24" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>47</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1637,21 +1640,21 @@
         <v>0.65600000000000003</v>
       </c>
       <c r="F25" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G25" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H25" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -1667,21 +1670,21 @@
         <v>6.82</v>
       </c>
       <c r="F26" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G26" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H26" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1697,21 +1700,21 @@
         <v>3.92</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G27" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H27" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1727,21 +1730,21 @@
         <v>12.95</v>
       </c>
       <c r="F28" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G28" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H28" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1757,21 +1760,21 @@
         <v>10.95</v>
       </c>
       <c r="F29" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G29" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H29" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1787,21 +1790,21 @@
         <v>0.33200000000000002</v>
       </c>
       <c r="F30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1817,21 +1820,21 @@
         <v>4.51</v>
       </c>
       <c r="F31" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G31" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H31" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1847,21 +1850,21 @@
         <v>2.95</v>
       </c>
       <c r="F32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H32" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1877,21 +1880,21 @@
         <v>0.62</v>
       </c>
       <c r="F33" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G33" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H33" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1907,21 +1910,21 @@
         <v>9.82</v>
       </c>
       <c r="F34" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G34" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H34" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -1937,21 +1940,21 @@
         <v>0.99119999999999997</v>
       </c>
       <c r="F35" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G35" s="4">
         <v>0.1</v>
       </c>
       <c r="H35" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1967,21 +1970,21 @@
         <v>1.1457599999999999</v>
       </c>
       <c r="F36" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G36" s="4">
         <v>0.2</v>
       </c>
       <c r="H36" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -1997,21 +2000,21 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="F37" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G37" s="4">
         <v>0.01</v>
       </c>
       <c r="H37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -2027,21 +2030,21 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="F38" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G38" s="4">
         <v>0.01</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -2057,21 +2060,21 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="F39" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G39" s="4">
         <v>0.01</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B40">
         <v>6</v>
@@ -2087,21 +2090,21 @@
         <v>0.126</v>
       </c>
       <c r="F40" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G40" s="4">
         <v>0.01</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -2117,21 +2120,21 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="F41" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G41" s="4">
         <v>0.01</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B42">
         <v>6</v>
@@ -2147,21 +2150,21 @@
         <v>0.126</v>
       </c>
       <c r="F42" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G42" s="4">
         <v>0.01</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -2177,24 +2180,24 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F43" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G43" s="4">
         <v>0.01</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B44">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C44">
         <v>0.15</v>
@@ -2204,24 +2207,24 @@
       </c>
       <c r="E44">
         <f t="shared" ref="E44:E49" si="5">D44*B44</f>
-        <v>0.67200000000000004</v>
+        <v>0.71400000000000008</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G44" s="4">
         <v>0.01</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B45">
         <v>20</v>
@@ -2237,21 +2240,21 @@
         <v>0.48</v>
       </c>
       <c r="F45" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G45" s="4">
         <v>0.01</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2267,21 +2270,21 @@
         <v>1.62</v>
       </c>
       <c r="F46" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G46" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H46" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B47">
         <v>22</v>
@@ -2297,21 +2300,21 @@
         <v>3.4980000000000002</v>
       </c>
       <c r="F47" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G47" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H47" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B48">
         <v>4</v>
@@ -2327,21 +2330,21 @@
         <v>0.312</v>
       </c>
       <c r="F48" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G48" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H48" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B49">
         <v>5</v>
@@ -2357,71 +2360,66 @@
         <v>8.1499999999999986</v>
       </c>
       <c r="F49" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G49" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H49" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I8" r:id="rId1" xr:uid="{492E2148-F2AF-4459-8BA6-A859737F68D7}"/>
-    <hyperlink ref="I12" r:id="rId2" xr:uid="{0D24AB4C-ECAE-42C1-8B77-5510569F6787}"/>
-    <hyperlink ref="I9" r:id="rId3" xr:uid="{0017AB32-864D-4EAE-A238-CC8C9ECE97E1}"/>
-    <hyperlink ref="I11" r:id="rId4" xr:uid="{810A7E28-8D43-49AE-85FF-C23B6546A59B}"/>
-    <hyperlink ref="I10" r:id="rId5" xr:uid="{C6ED980E-7D4F-4DED-9C1A-FD67E374B9EA}"/>
-    <hyperlink ref="I2" r:id="rId6" xr:uid="{DF430ECF-0197-4C9E-9BD2-379127E51230}"/>
-    <hyperlink ref="I3" r:id="rId7" xr:uid="{2AF31FA7-48C2-4C74-97F6-C262279C839A}"/>
-    <hyperlink ref="I14" r:id="rId8" xr:uid="{5C7B7096-C592-427C-AC61-D40625D2193E}"/>
-    <hyperlink ref="I13" r:id="rId9" xr:uid="{5910EA08-9E19-4F72-9ADB-C3DC943A9880}"/>
-    <hyperlink ref="I15" r:id="rId10" xr:uid="{63A18238-7A07-49F3-A985-3D844C29C2CB}"/>
-    <hyperlink ref="I17" r:id="rId11" xr:uid="{2E91CEEF-D030-42BD-8B62-5BA748F4BFB7}"/>
-    <hyperlink ref="I18" r:id="rId12" xr:uid="{C09D32E1-5978-432C-95AA-B215B3A36ED3}"/>
-    <hyperlink ref="I19" r:id="rId13" xr:uid="{710A736C-147F-44A6-980D-F8ED04995C2A}"/>
-    <hyperlink ref="I23" r:id="rId14" xr:uid="{92C36C49-CEB7-4A72-B877-A11899E89BE2}"/>
-    <hyperlink ref="I25" r:id="rId15" xr:uid="{4EB0278A-4B3D-430B-A61C-80C7370DCF6F}"/>
-    <hyperlink ref="I24" r:id="rId16" xr:uid="{BF6DE5DC-89C2-4BD8-AE62-76723EEEDE83}"/>
-    <hyperlink ref="I26" r:id="rId17" xr:uid="{486F8D7D-0B15-47C5-9D97-1AA471F91B5D}"/>
-    <hyperlink ref="I27" r:id="rId18" xr:uid="{D136844E-AA85-4E69-B0DA-01D3AFD45890}"/>
-    <hyperlink ref="I20" r:id="rId19" xr:uid="{5938C70C-9994-491E-8C8E-714909A51FC5}"/>
-    <hyperlink ref="I21" r:id="rId20" xr:uid="{09D08152-5192-4B18-A262-9992FC42F93A}"/>
-    <hyperlink ref="I31" r:id="rId21" xr:uid="{8C33B197-A161-4837-82ED-5B68E46D5DF7}"/>
-    <hyperlink ref="I32" r:id="rId22" xr:uid="{F3FBB0A4-3902-4DAF-A37B-76F301E09156}"/>
-    <hyperlink ref="I33" r:id="rId23" xr:uid="{AFE4F09A-555F-42AA-B131-38F6ED42FEB3}"/>
-    <hyperlink ref="I34" r:id="rId24" xr:uid="{023AC9E4-D4A9-4F9F-A849-E84F4EC49E5C}"/>
-    <hyperlink ref="I37" r:id="rId25" xr:uid="{09D3FEA4-5ABC-4407-99EB-DFD5FEF8F848}"/>
-    <hyperlink ref="I38" r:id="rId26" xr:uid="{9FC6225D-D32E-4A1B-BCB1-3C48474CD21B}"/>
-    <hyperlink ref="I16" r:id="rId27" xr:uid="{BDD89C76-645C-4FB0-A077-0F3054C86712}"/>
-    <hyperlink ref="I39" r:id="rId28" xr:uid="{B2D7D052-A1D1-415D-B230-8957BB283201}"/>
-    <hyperlink ref="I40" r:id="rId29" xr:uid="{250A83A0-C654-4E28-9F2F-BD3ADC2DD1C3}"/>
-    <hyperlink ref="I41" r:id="rId30" xr:uid="{D3DFAAE9-3735-43A8-8793-71C985FB4FBD}"/>
-    <hyperlink ref="I42" r:id="rId31" xr:uid="{19ECA42A-A782-4EA0-882E-A4E617FFCBC6}"/>
-    <hyperlink ref="I43" r:id="rId32" xr:uid="{B9D01495-AA86-4548-AD27-CA6C7A678A28}"/>
-    <hyperlink ref="I45" r:id="rId33" xr:uid="{8B3B765E-E142-444F-8ED5-BEFBF459EAEB}"/>
-    <hyperlink ref="I44" r:id="rId34" xr:uid="{76DF0F02-5C82-45C2-9680-F9E4B8763809}"/>
-    <hyperlink ref="I22" r:id="rId35" xr:uid="{D821FAF4-4519-4BDF-80AB-0EB42CE5E00D}"/>
-    <hyperlink ref="I28" r:id="rId36" xr:uid="{C61A3691-2C87-47DA-B2B4-576CC8E7A68B}"/>
-    <hyperlink ref="I29" r:id="rId37" xr:uid="{C6FD9A6B-9214-438C-AE3A-BEB73598759E}"/>
-    <hyperlink ref="I36" r:id="rId38" display="https://www.digikey.com/en/products/detail/sumida-america-inc/CDMC6D28NP-4R7MC/2620811?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALAAxwDMdIAuoQA4AuUIAymwE4CWAOwDmIAL6EwAJhmIQKSBhwFiZcAAIAsgAkAXk1YdIIAKqD%2BbAPKpNudNgCuvXOMJSqADgDschUryEJJDkFAB0XuoArdoGIOycZhbWtvZOLhIgALRSvlB8DipB5ACsTBmZENDyaFgBqsEgtJ5lYmJAA" xr:uid="{834AE210-016B-4CBE-8EA6-536982F867F8}"/>
-    <hyperlink ref="I6" r:id="rId39" xr:uid="{5FEB1D7B-ABF4-46FC-B2BF-C149C38A6E15}"/>
-    <hyperlink ref="I7" r:id="rId40" xr:uid="{3E12A4D2-1E68-4814-9E5C-4A39C2A05CAA}"/>
-    <hyperlink ref="I30" r:id="rId41" xr:uid="{71BD25B4-F05D-4E5F-BBE0-AED2073FD801}"/>
-    <hyperlink ref="I35" r:id="rId42" xr:uid="{11E1F2A9-A652-467C-9ED3-0A573DF4D4AE}"/>
-    <hyperlink ref="I4" r:id="rId43" xr:uid="{CFFFBE4E-F764-4212-90C8-68835B2878A6}"/>
-    <hyperlink ref="I5" r:id="rId44" xr:uid="{96128D2E-BBA5-41CE-AC6A-1AA6E9FE18A4}"/>
-    <hyperlink ref="I46" r:id="rId45" xr:uid="{A5DA30F9-7BF1-4C3E-B54C-251DEC8F6CA5}"/>
-    <hyperlink ref="I47" r:id="rId46" xr:uid="{0D1F7C52-82CE-47F5-BED9-561932209F4B}"/>
-    <hyperlink ref="I48" r:id="rId47" xr:uid="{403DED07-E041-48A3-A5DB-05F6E1A94F4D}"/>
-    <hyperlink ref="I49" r:id="rId48" xr:uid="{D6866B2B-F4EF-43C9-BD38-9E3E21900AD2}"/>
+    <hyperlink ref="I12" r:id="rId1" xr:uid="{0D24AB4C-ECAE-42C1-8B77-5510569F6787}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{DF430ECF-0197-4C9E-9BD2-379127E51230}"/>
+    <hyperlink ref="I3" r:id="rId3" xr:uid="{2AF31FA7-48C2-4C74-97F6-C262279C839A}"/>
+    <hyperlink ref="I14" r:id="rId4" xr:uid="{5C7B7096-C592-427C-AC61-D40625D2193E}"/>
+    <hyperlink ref="I13" r:id="rId5" xr:uid="{5910EA08-9E19-4F72-9ADB-C3DC943A9880}"/>
+    <hyperlink ref="I15" r:id="rId6" xr:uid="{63A18238-7A07-49F3-A985-3D844C29C2CB}"/>
+    <hyperlink ref="I17" r:id="rId7" xr:uid="{2E91CEEF-D030-42BD-8B62-5BA748F4BFB7}"/>
+    <hyperlink ref="I18" r:id="rId8" xr:uid="{C09D32E1-5978-432C-95AA-B215B3A36ED3}"/>
+    <hyperlink ref="I19" r:id="rId9" xr:uid="{710A736C-147F-44A6-980D-F8ED04995C2A}"/>
+    <hyperlink ref="I23" r:id="rId10" xr:uid="{92C36C49-CEB7-4A72-B877-A11899E89BE2}"/>
+    <hyperlink ref="I25" r:id="rId11" xr:uid="{4EB0278A-4B3D-430B-A61C-80C7370DCF6F}"/>
+    <hyperlink ref="I26" r:id="rId12" xr:uid="{486F8D7D-0B15-47C5-9D97-1AA471F91B5D}"/>
+    <hyperlink ref="I27" r:id="rId13" xr:uid="{D136844E-AA85-4E69-B0DA-01D3AFD45890}"/>
+    <hyperlink ref="I20" r:id="rId14" xr:uid="{5938C70C-9994-491E-8C8E-714909A51FC5}"/>
+    <hyperlink ref="I21" r:id="rId15" xr:uid="{09D08152-5192-4B18-A262-9992FC42F93A}"/>
+    <hyperlink ref="I31" r:id="rId16" xr:uid="{8C33B197-A161-4837-82ED-5B68E46D5DF7}"/>
+    <hyperlink ref="I32" r:id="rId17" xr:uid="{F3FBB0A4-3902-4DAF-A37B-76F301E09156}"/>
+    <hyperlink ref="I33" r:id="rId18" xr:uid="{AFE4F09A-555F-42AA-B131-38F6ED42FEB3}"/>
+    <hyperlink ref="I34" r:id="rId19" xr:uid="{023AC9E4-D4A9-4F9F-A849-E84F4EC49E5C}"/>
+    <hyperlink ref="I37" r:id="rId20" xr:uid="{09D3FEA4-5ABC-4407-99EB-DFD5FEF8F848}"/>
+    <hyperlink ref="I38" r:id="rId21" xr:uid="{9FC6225D-D32E-4A1B-BCB1-3C48474CD21B}"/>
+    <hyperlink ref="I16" r:id="rId22" xr:uid="{BDD89C76-645C-4FB0-A077-0F3054C86712}"/>
+    <hyperlink ref="I39" r:id="rId23" xr:uid="{B2D7D052-A1D1-415D-B230-8957BB283201}"/>
+    <hyperlink ref="I40" r:id="rId24" xr:uid="{250A83A0-C654-4E28-9F2F-BD3ADC2DD1C3}"/>
+    <hyperlink ref="I41" r:id="rId25" xr:uid="{D3DFAAE9-3735-43A8-8793-71C985FB4FBD}"/>
+    <hyperlink ref="I42" r:id="rId26" xr:uid="{19ECA42A-A782-4EA0-882E-A4E617FFCBC6}"/>
+    <hyperlink ref="I43" r:id="rId27" xr:uid="{B9D01495-AA86-4548-AD27-CA6C7A678A28}"/>
+    <hyperlink ref="I45" r:id="rId28" xr:uid="{8B3B765E-E142-444F-8ED5-BEFBF459EAEB}"/>
+    <hyperlink ref="I44" r:id="rId29" xr:uid="{76DF0F02-5C82-45C2-9680-F9E4B8763809}"/>
+    <hyperlink ref="I22" r:id="rId30" xr:uid="{D821FAF4-4519-4BDF-80AB-0EB42CE5E00D}"/>
+    <hyperlink ref="I28" r:id="rId31" xr:uid="{C61A3691-2C87-47DA-B2B4-576CC8E7A68B}"/>
+    <hyperlink ref="I29" r:id="rId32" xr:uid="{C6FD9A6B-9214-438C-AE3A-BEB73598759E}"/>
+    <hyperlink ref="I36" r:id="rId33" display="https://www.digikey.com/en/products/detail/sumida-america-inc/CDMC6D28NP-4R7MC/2620811?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALAAxwDMdIAuoQA4AuUIAymwE4CWAOwDmIAL6EwAJhmIQKSBhwFiZcAAIAsgAkAXk1YdIIAKqD%2BbAPKpNudNgCuvXOMJSqADgDschUryEJJDkFAB0XuoArdoGIOycZhbWtvZOLhIgALRSvlB8DipB5ACsTBmZENDyaFgBqsEgtJ5lYmJAA" xr:uid="{834AE210-016B-4CBE-8EA6-536982F867F8}"/>
+    <hyperlink ref="I6" r:id="rId34" xr:uid="{5FEB1D7B-ABF4-46FC-B2BF-C149C38A6E15}"/>
+    <hyperlink ref="I7" r:id="rId35" xr:uid="{3E12A4D2-1E68-4814-9E5C-4A39C2A05CAA}"/>
+    <hyperlink ref="I30" r:id="rId36" xr:uid="{71BD25B4-F05D-4E5F-BBE0-AED2073FD801}"/>
+    <hyperlink ref="I35" r:id="rId37" xr:uid="{11E1F2A9-A652-467C-9ED3-0A573DF4D4AE}"/>
+    <hyperlink ref="I4" r:id="rId38" xr:uid="{CFFFBE4E-F764-4212-90C8-68835B2878A6}"/>
+    <hyperlink ref="I5" r:id="rId39" xr:uid="{96128D2E-BBA5-41CE-AC6A-1AA6E9FE18A4}"/>
+    <hyperlink ref="I46" r:id="rId40" xr:uid="{A5DA30F9-7BF1-4C3E-B54C-251DEC8F6CA5}"/>
+    <hyperlink ref="I47" r:id="rId41" xr:uid="{0D1F7C52-82CE-47F5-BED9-561932209F4B}"/>
+    <hyperlink ref="I48" r:id="rId42" xr:uid="{403DED07-E041-48A3-A5DB-05F6E1A94F4D}"/>
+    <hyperlink ref="I49" r:id="rId43" xr:uid="{D6866B2B-F4EF-43C9-BD38-9E3E21900AD2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId49"/>
+  <pageSetup orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed grid size, began regrouping
</commit_message>
<xml_diff>
--- a/Part List.xlsx
+++ b/Part List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krotain\Documents\git\493\ece_492-3_topic_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1985A8ED-AE36-4DB6-94D6-DC1F3D97C7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E88120C-FC4C-4568-847D-B5EB4D0D51FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2175" windowWidth="29040" windowHeight="16440" xr2:uid="{DD9C814F-33BB-46B4-954A-62ACB4677A0F}"/>
   </bookViews>
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABF4B5B-D5F0-478D-961E-5722ED7FBC19}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed current sense and static modules
</commit_message>
<xml_diff>
--- a/Part List.xlsx
+++ b/Part List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krotain\Documents\git\493\ece_492-3_topic_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CB2FFD-E82C-46AC-8355-188006D20916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0128F763-5FE2-4057-B72E-03325D16634F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2175" windowWidth="29040" windowHeight="16440" xr2:uid="{DD9C814F-33BB-46B4-954A-62ACB4677A0F}"/>
   </bookViews>
@@ -251,15 +251,9 @@
     <t>https://www.mouser.com/ProductDetail/Ohmite/KDV06FR180ET?qs=l4Gc20tDgJLuG9Oc1mkpPg%3D%3D</t>
   </si>
   <si>
-    <t>KDV06FR300ET</t>
-  </si>
-  <si>
     <t>300mOhm</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Ohmite/KDV06FR300ET?qs=l4Gc20tDgJIqinXnKONtAA%3D%3D</t>
-  </si>
-  <si>
     <t>SDR03EZPF1002</t>
   </si>
   <si>
@@ -507,6 +501,12 @@
   </si>
   <si>
     <t>HC-49/US-SM</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Ohmite/KDV12FR300ET?qs=l4Gc20tDgJJqdOINs5xdYg%3D%3D</t>
+  </si>
+  <si>
+    <t>KDV12FR300ET</t>
   </si>
 </sst>
 </file>
@@ -887,7 +887,7 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +901,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -928,7 +928,7 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -962,7 +962,7 @@
       </c>
       <c r="J2">
         <f>SUM(E:E)</f>
-        <v>84.765760000000057</v>
+        <v>84.781760000000048</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -997,7 +997,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1013,21 +1013,21 @@
         <v>4.04</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G4" s="4">
         <v>0.2</v>
       </c>
       <c r="H4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1043,21 +1043,21 @@
         <v>0.874</v>
       </c>
       <c r="F5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G5" s="4">
         <v>0.2</v>
       </c>
       <c r="H5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1073,21 +1073,21 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G6" s="4">
         <v>0.2</v>
       </c>
       <c r="H6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1103,16 +1103,16 @@
         <v>0.36</v>
       </c>
       <c r="F7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G7" s="4">
         <v>0.2</v>
       </c>
       <c r="H7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1139,15 +1139,15 @@
         <v>0.1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -1169,15 +1169,15 @@
         <v>0.1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1202,12 +1202,12 @@
         <v>17</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1232,12 +1232,12 @@
         <v>17</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B12">
         <v>9</v>
@@ -1262,12 +1262,12 @@
         <v>63</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -1292,12 +1292,12 @@
         <v>63</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1322,12 +1322,12 @@
         <v>63</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1352,7 +1352,7 @@
         <v>63</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1537,7 +1537,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -1559,10 +1559,10 @@
         <v>28</v>
       </c>
       <c r="H22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1619,10 +1619,10 @@
         <v>28</v>
       </c>
       <c r="H24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1717,7 +1717,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1742,12 +1742,12 @@
         <v>28</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1772,12 +1772,12 @@
         <v>28</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1802,7 +1802,7 @@
         <v>28</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1867,7 +1867,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1889,10 +1889,10 @@
         <v>28</v>
       </c>
       <c r="H33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1927,7 +1927,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -1949,15 +1949,15 @@
         <v>0.1</v>
       </c>
       <c r="H35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -1973,16 +1973,16 @@
         <v>1.1457599999999999</v>
       </c>
       <c r="F36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G36" s="4">
         <v>0.2</v>
       </c>
       <c r="H36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2017,37 +2017,37 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>156</v>
       </c>
       <c r="B38">
         <v>2</v>
       </c>
       <c r="C38">
-        <v>0.26</v>
+        <v>0.31</v>
       </c>
       <c r="D38">
-        <v>3.5999999999999997E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="E38">
         <f t="shared" si="4"/>
-        <v>7.1999999999999995E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="F38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G38" s="4">
         <v>0.01</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>63</v>
+        <v>149</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -2063,7 +2063,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="F39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G39" s="4">
         <v>0.01</v>
@@ -2072,12 +2072,12 @@
         <v>63</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B40">
         <v>6</v>
@@ -2093,7 +2093,7 @@
         <v>0.126</v>
       </c>
       <c r="F40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G40" s="4">
         <v>0.01</v>
@@ -2102,12 +2102,12 @@
         <v>63</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -2123,7 +2123,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="F41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G41" s="4">
         <v>0.01</v>
@@ -2132,12 +2132,12 @@
         <v>63</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B42">
         <v>6</v>
@@ -2153,7 +2153,7 @@
         <v>0.126</v>
       </c>
       <c r="F42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G42" s="4">
         <v>0.01</v>
@@ -2162,12 +2162,12 @@
         <v>63</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -2183,7 +2183,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F43" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G43" s="4">
         <v>0.01</v>
@@ -2192,12 +2192,12 @@
         <v>63</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B44">
         <v>34</v>
@@ -2213,7 +2213,7 @@
         <v>0.71400000000000008</v>
       </c>
       <c r="F44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G44" s="4">
         <v>0.01</v>
@@ -2222,12 +2222,12 @@
         <v>63</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B45">
         <v>20</v>
@@ -2243,7 +2243,7 @@
         <v>0.48</v>
       </c>
       <c r="F45" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G45" s="4">
         <v>0.01</v>
@@ -2252,12 +2252,12 @@
         <v>63</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2282,12 +2282,12 @@
         <v>28</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B47">
         <v>22</v>
@@ -2312,12 +2312,12 @@
         <v>28</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B48">
         <v>4</v>
@@ -2342,12 +2342,12 @@
         <v>28</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B49">
         <v>5</v>
@@ -2372,7 +2372,7 @@
         <v>28</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2397,31 +2397,31 @@
     <hyperlink ref="I32" r:id="rId17" xr:uid="{F3FBB0A4-3902-4DAF-A37B-76F301E09156}"/>
     <hyperlink ref="I34" r:id="rId18" xr:uid="{023AC9E4-D4A9-4F9F-A849-E84F4EC49E5C}"/>
     <hyperlink ref="I37" r:id="rId19" xr:uid="{09D3FEA4-5ABC-4407-99EB-DFD5FEF8F848}"/>
-    <hyperlink ref="I38" r:id="rId20" xr:uid="{9FC6225D-D32E-4A1B-BCB1-3C48474CD21B}"/>
-    <hyperlink ref="I16" r:id="rId21" xr:uid="{BDD89C76-645C-4FB0-A077-0F3054C86712}"/>
-    <hyperlink ref="I39" r:id="rId22" xr:uid="{B2D7D052-A1D1-415D-B230-8957BB283201}"/>
-    <hyperlink ref="I40" r:id="rId23" xr:uid="{250A83A0-C654-4E28-9F2F-BD3ADC2DD1C3}"/>
-    <hyperlink ref="I41" r:id="rId24" xr:uid="{D3DFAAE9-3735-43A8-8793-71C985FB4FBD}"/>
-    <hyperlink ref="I42" r:id="rId25" xr:uid="{19ECA42A-A782-4EA0-882E-A4E617FFCBC6}"/>
-    <hyperlink ref="I43" r:id="rId26" xr:uid="{B9D01495-AA86-4548-AD27-CA6C7A678A28}"/>
-    <hyperlink ref="I45" r:id="rId27" xr:uid="{8B3B765E-E142-444F-8ED5-BEFBF459EAEB}"/>
-    <hyperlink ref="I44" r:id="rId28" xr:uid="{76DF0F02-5C82-45C2-9680-F9E4B8763809}"/>
-    <hyperlink ref="I22" r:id="rId29" xr:uid="{D821FAF4-4519-4BDF-80AB-0EB42CE5E00D}"/>
-    <hyperlink ref="I28" r:id="rId30" xr:uid="{C61A3691-2C87-47DA-B2B4-576CC8E7A68B}"/>
-    <hyperlink ref="I29" r:id="rId31" xr:uid="{C6FD9A6B-9214-438C-AE3A-BEB73598759E}"/>
-    <hyperlink ref="I36" r:id="rId32" display="https://www.digikey.com/en/products/detail/sumida-america-inc/CDMC6D28NP-4R7MC/2620811?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALAAxwDMdIAuoQA4AuUIAymwE4CWAOwDmIAL6EwAJhmIQKSBhwFiZcAAIAsgAkAXk1YdIIAKqD%2BbAPKpNudNgCuvXOMJSqADgDschUryEJJDkFAB0XuoArdoGIOycZhbWtvZOLhIgALRSvlB8DipB5ACsTBmZENDyaFgBqsEgtJ5lYmJAA" xr:uid="{834AE210-016B-4CBE-8EA6-536982F867F8}"/>
-    <hyperlink ref="I6" r:id="rId33" xr:uid="{5FEB1D7B-ABF4-46FC-B2BF-C149C38A6E15}"/>
-    <hyperlink ref="I7" r:id="rId34" xr:uid="{3E12A4D2-1E68-4814-9E5C-4A39C2A05CAA}"/>
-    <hyperlink ref="I30" r:id="rId35" xr:uid="{71BD25B4-F05D-4E5F-BBE0-AED2073FD801}"/>
-    <hyperlink ref="I35" r:id="rId36" xr:uid="{11E1F2A9-A652-467C-9ED3-0A573DF4D4AE}"/>
-    <hyperlink ref="I4" r:id="rId37" xr:uid="{CFFFBE4E-F764-4212-90C8-68835B2878A6}"/>
-    <hyperlink ref="I5" r:id="rId38" xr:uid="{96128D2E-BBA5-41CE-AC6A-1AA6E9FE18A4}"/>
-    <hyperlink ref="I46" r:id="rId39" xr:uid="{A5DA30F9-7BF1-4C3E-B54C-251DEC8F6CA5}"/>
-    <hyperlink ref="I47" r:id="rId40" xr:uid="{0D1F7C52-82CE-47F5-BED9-561932209F4B}"/>
-    <hyperlink ref="I48" r:id="rId41" xr:uid="{403DED07-E041-48A3-A5DB-05F6E1A94F4D}"/>
-    <hyperlink ref="I49" r:id="rId42" xr:uid="{D6866B2B-F4EF-43C9-BD38-9E3E21900AD2}"/>
-    <hyperlink ref="I8" r:id="rId43" xr:uid="{13230959-78D1-4DC9-AB13-5D1095CF6E0B}"/>
-    <hyperlink ref="I24" r:id="rId44" xr:uid="{89824DF9-7F8D-4EDA-B5FC-F48A77F4E608}"/>
+    <hyperlink ref="I16" r:id="rId20" xr:uid="{BDD89C76-645C-4FB0-A077-0F3054C86712}"/>
+    <hyperlink ref="I39" r:id="rId21" xr:uid="{B2D7D052-A1D1-415D-B230-8957BB283201}"/>
+    <hyperlink ref="I40" r:id="rId22" xr:uid="{250A83A0-C654-4E28-9F2F-BD3ADC2DD1C3}"/>
+    <hyperlink ref="I41" r:id="rId23" xr:uid="{D3DFAAE9-3735-43A8-8793-71C985FB4FBD}"/>
+    <hyperlink ref="I42" r:id="rId24" xr:uid="{19ECA42A-A782-4EA0-882E-A4E617FFCBC6}"/>
+    <hyperlink ref="I43" r:id="rId25" xr:uid="{B9D01495-AA86-4548-AD27-CA6C7A678A28}"/>
+    <hyperlink ref="I45" r:id="rId26" xr:uid="{8B3B765E-E142-444F-8ED5-BEFBF459EAEB}"/>
+    <hyperlink ref="I44" r:id="rId27" xr:uid="{76DF0F02-5C82-45C2-9680-F9E4B8763809}"/>
+    <hyperlink ref="I22" r:id="rId28" xr:uid="{D821FAF4-4519-4BDF-80AB-0EB42CE5E00D}"/>
+    <hyperlink ref="I28" r:id="rId29" xr:uid="{C61A3691-2C87-47DA-B2B4-576CC8E7A68B}"/>
+    <hyperlink ref="I29" r:id="rId30" xr:uid="{C6FD9A6B-9214-438C-AE3A-BEB73598759E}"/>
+    <hyperlink ref="I36" r:id="rId31" display="https://www.digikey.com/en/products/detail/sumida-america-inc/CDMC6D28NP-4R7MC/2620811?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALAAxwDMdIAuoQA4AuUIAymwE4CWAOwDmIAL6EwAJhmIQKSBhwFiZcAAIAsgAkAXk1YdIIAKqD%2BbAPKpNudNgCuvXOMJSqADgDschUryEJJDkFAB0XuoArdoGIOycZhbWtvZOLhIgALRSvlB8DipB5ACsTBmZENDyaFgBqsEgtJ5lYmJAA" xr:uid="{834AE210-016B-4CBE-8EA6-536982F867F8}"/>
+    <hyperlink ref="I6" r:id="rId32" xr:uid="{5FEB1D7B-ABF4-46FC-B2BF-C149C38A6E15}"/>
+    <hyperlink ref="I7" r:id="rId33" xr:uid="{3E12A4D2-1E68-4814-9E5C-4A39C2A05CAA}"/>
+    <hyperlink ref="I30" r:id="rId34" xr:uid="{71BD25B4-F05D-4E5F-BBE0-AED2073FD801}"/>
+    <hyperlink ref="I35" r:id="rId35" xr:uid="{11E1F2A9-A652-467C-9ED3-0A573DF4D4AE}"/>
+    <hyperlink ref="I4" r:id="rId36" xr:uid="{CFFFBE4E-F764-4212-90C8-68835B2878A6}"/>
+    <hyperlink ref="I5" r:id="rId37" xr:uid="{96128D2E-BBA5-41CE-AC6A-1AA6E9FE18A4}"/>
+    <hyperlink ref="I46" r:id="rId38" xr:uid="{A5DA30F9-7BF1-4C3E-B54C-251DEC8F6CA5}"/>
+    <hyperlink ref="I47" r:id="rId39" xr:uid="{0D1F7C52-82CE-47F5-BED9-561932209F4B}"/>
+    <hyperlink ref="I48" r:id="rId40" xr:uid="{403DED07-E041-48A3-A5DB-05F6E1A94F4D}"/>
+    <hyperlink ref="I49" r:id="rId41" xr:uid="{D6866B2B-F4EF-43C9-BD38-9E3E21900AD2}"/>
+    <hyperlink ref="I8" r:id="rId42" xr:uid="{13230959-78D1-4DC9-AB13-5D1095CF6E0B}"/>
+    <hyperlink ref="I24" r:id="rId43" xr:uid="{89824DF9-7F8D-4EDA-B5FC-F48A77F4E608}"/>
+    <hyperlink ref="I38" r:id="rId44" xr:uid="{024C97FE-9878-433D-AD7C-9C1B67A9EF58}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId45"/>

</xml_diff>

<commit_message>
Fixed MCU communication pins and optocoupler
</commit_message>
<xml_diff>
--- a/Part List.xlsx
+++ b/Part List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krotain\Documents\git\493\ece_492-3_topic_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0128F763-5FE2-4057-B72E-03325D16634F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22072091-6EAE-4AF4-A4C9-A037E10F6F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2175" windowWidth="29040" windowHeight="16440" xr2:uid="{DD9C814F-33BB-46B4-954A-62ACB4677A0F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="163">
   <si>
     <t>Quantity</t>
   </si>
@@ -507,6 +507,24 @@
   </si>
   <si>
     <t>KDV12FR300ET</t>
+  </si>
+  <si>
+    <t>ESR03EZPF22R0</t>
+  </si>
+  <si>
+    <t>22Ohm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF22R0?qs=493kPxzlxfL2v77xEtzYQA%3D%3D</t>
+  </si>
+  <si>
+    <t>ESR03EZPF4700</t>
+  </si>
+  <si>
+    <t>470Ohm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF4700?qs=DyUWGjl%252BcVsZQGp8SgvEfA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -884,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABF4B5B-D5F0-478D-961E-5722ED7FBC19}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,7 +980,7 @@
       </c>
       <c r="J2">
         <f>SUM(E:E)</f>
-        <v>84.781760000000048</v>
+        <v>84.873760000000061</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2257,80 +2275,80 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46">
-        <v>2.69</v>
+        <v>0.16</v>
       </c>
       <c r="D46">
-        <v>1.62</v>
+        <v>2.3E-2</v>
       </c>
       <c r="E46">
         <f t="shared" si="5"/>
-        <v>1.62</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="F46" t="s">
-        <v>28</v>
-      </c>
-      <c r="G46" t="s">
-        <v>28</v>
-      </c>
-      <c r="H46" t="s">
-        <v>28</v>
+        <v>161</v>
+      </c>
+      <c r="G46" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="B47">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C47">
-        <v>0.27</v>
+        <v>0.16</v>
       </c>
       <c r="D47">
-        <v>0.159</v>
+        <v>2.3E-2</v>
       </c>
       <c r="E47">
-        <f t="shared" si="5"/>
-        <v>3.4980000000000002</v>
+        <f>D47*B47</f>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="F47" t="s">
-        <v>28</v>
-      </c>
-      <c r="G47" t="s">
-        <v>28</v>
-      </c>
-      <c r="H47" t="s">
-        <v>28</v>
+        <v>158</v>
+      </c>
+      <c r="G47" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <v>0.2</v>
+        <v>2.69</v>
       </c>
       <c r="D48">
-        <v>7.8E-2</v>
+        <v>1.62</v>
       </c>
       <c r="E48">
-        <f t="shared" si="5"/>
-        <v>0.312</v>
+        <f>D48*B48</f>
+        <v>1.62</v>
       </c>
       <c r="F48" t="s">
         <v>28</v>
@@ -2342,36 +2360,96 @@
         <v>28</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49">
+        <v>22</v>
+      </c>
+      <c r="C49">
+        <v>0.27</v>
+      </c>
+      <c r="D49">
+        <v>0.159</v>
+      </c>
+      <c r="E49">
+        <f>D49*B49</f>
+        <v>3.4980000000000002</v>
+      </c>
+      <c r="F49" t="s">
+        <v>28</v>
+      </c>
+      <c r="G49" t="s">
+        <v>28</v>
+      </c>
+      <c r="H49" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>138</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>0.2</v>
+      </c>
+      <c r="D50">
+        <v>7.8E-2</v>
+      </c>
+      <c r="E50">
+        <f>D50*B50</f>
+        <v>0.312</v>
+      </c>
+      <c r="F50" t="s">
+        <v>28</v>
+      </c>
+      <c r="G50" t="s">
+        <v>28</v>
+      </c>
+      <c r="H50" t="s">
+        <v>28</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>141</v>
       </c>
-      <c r="B49">
+      <c r="B51">
         <v>5</v>
       </c>
-      <c r="C49">
+      <c r="C51">
         <v>2.36</v>
       </c>
-      <c r="D49">
+      <c r="D51">
         <v>1.63</v>
       </c>
-      <c r="E49">
-        <f t="shared" si="5"/>
+      <c r="E51">
+        <f>D51*B51</f>
         <v>8.1499999999999986</v>
       </c>
-      <c r="F49" t="s">
-        <v>28</v>
-      </c>
-      <c r="G49" t="s">
-        <v>28</v>
-      </c>
-      <c r="H49" t="s">
-        <v>28</v>
-      </c>
-      <c r="I49" s="3" t="s">
+      <c r="F51" t="s">
+        <v>28</v>
+      </c>
+      <c r="G51" t="s">
+        <v>28</v>
+      </c>
+      <c r="H51" t="s">
+        <v>28</v>
+      </c>
+      <c r="I51" s="3" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2415,15 +2493,17 @@
     <hyperlink ref="I35" r:id="rId35" xr:uid="{11E1F2A9-A652-467C-9ED3-0A573DF4D4AE}"/>
     <hyperlink ref="I4" r:id="rId36" xr:uid="{CFFFBE4E-F764-4212-90C8-68835B2878A6}"/>
     <hyperlink ref="I5" r:id="rId37" xr:uid="{96128D2E-BBA5-41CE-AC6A-1AA6E9FE18A4}"/>
-    <hyperlink ref="I46" r:id="rId38" xr:uid="{A5DA30F9-7BF1-4C3E-B54C-251DEC8F6CA5}"/>
-    <hyperlink ref="I47" r:id="rId39" xr:uid="{0D1F7C52-82CE-47F5-BED9-561932209F4B}"/>
-    <hyperlink ref="I48" r:id="rId40" xr:uid="{403DED07-E041-48A3-A5DB-05F6E1A94F4D}"/>
-    <hyperlink ref="I49" r:id="rId41" xr:uid="{D6866B2B-F4EF-43C9-BD38-9E3E21900AD2}"/>
+    <hyperlink ref="I48" r:id="rId38" xr:uid="{A5DA30F9-7BF1-4C3E-B54C-251DEC8F6CA5}"/>
+    <hyperlink ref="I49" r:id="rId39" xr:uid="{0D1F7C52-82CE-47F5-BED9-561932209F4B}"/>
+    <hyperlink ref="I50" r:id="rId40" xr:uid="{403DED07-E041-48A3-A5DB-05F6E1A94F4D}"/>
+    <hyperlink ref="I51" r:id="rId41" xr:uid="{D6866B2B-F4EF-43C9-BD38-9E3E21900AD2}"/>
     <hyperlink ref="I8" r:id="rId42" xr:uid="{13230959-78D1-4DC9-AB13-5D1095CF6E0B}"/>
     <hyperlink ref="I24" r:id="rId43" xr:uid="{89824DF9-7F8D-4EDA-B5FC-F48A77F4E608}"/>
     <hyperlink ref="I38" r:id="rId44" xr:uid="{024C97FE-9878-433D-AD7C-9C1B67A9EF58}"/>
+    <hyperlink ref="I47" r:id="rId45" xr:uid="{1DF79CBD-1538-440F-BACA-8832B5BAD705}"/>
+    <hyperlink ref="I46" r:id="rId46" xr:uid="{4934892E-6C0B-4AAD-AD47-1023163B958D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId45"/>
+  <pageSetup orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Front Panel Switch to the parts list
</commit_message>
<xml_diff>
--- a/Part List.xlsx
+++ b/Part List.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25825"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krotain\Documents\git\493\ece_492-3_topic_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4997CB-766E-4E7D-8422-EC8FB8FBE3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68F7F77F-9BFD-42F7-A6CA-E226824754F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43695" yWindow="2940" windowWidth="19395" windowHeight="13905" xr2:uid="{DD9C814F-33BB-46B4-954A-62ACB4677A0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="179">
+  <si>
+    <t>Part(*=Similar)</t>
+  </si>
   <si>
     <t>Quantity</t>
   </si>
@@ -53,72 +56,189 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Tolerance</t>
+  </si>
+  <si>
+    <t>Size/Package</t>
+  </si>
+  <si>
     <t>Link</t>
   </si>
   <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>PMEG3020CEP,115</t>
+  </si>
+  <si>
     <t>2A 30V</t>
   </si>
   <si>
+    <t>n/a</t>
+  </si>
+  <si>
     <t>SOD-128-2</t>
   </si>
   <si>
-    <t>Size/Package</t>
+    <t>https://www.mouser.com/ProductDetail/Nexperia/PMEG3020CEP115?qs=LMSg3oBIm%2Fgs8Me4yQ8MUQ%3D%3D</t>
+  </si>
+  <si>
+    <t>GS2A-LTP</t>
+  </si>
+  <si>
+    <t>2A 50V</t>
+  </si>
+  <si>
+    <t>DO-214AC-2</t>
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/Micro-Commercial-Components-MCC/GS2A-LTP?qs=sGAEpiMZZMtbRapU8LlZD8bHhgb8N%2FpPZyCVm66f8Yk%3D</t>
   </si>
   <si>
-    <t>GS2A-LTP</t>
-  </si>
-  <si>
-    <t>2A 50V</t>
-  </si>
-  <si>
-    <t>DO-214AC-2</t>
+    <t>UVR1E682MHD</t>
+  </si>
+  <si>
+    <t>6.8mF</t>
+  </si>
+  <si>
+    <t>18x35.5x7.5mm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Nichicon/UVR1E682MHD?qs=sGAEpiMZZMvwFf0viD3Y3UQjCBAmXhuzNEsRvpP9m3M%3D</t>
+  </si>
+  <si>
+    <t>UVZ1E102MPD</t>
+  </si>
+  <si>
+    <t>1mF</t>
+  </si>
+  <si>
+    <t>10x20x5mm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Nichicon/UVZ1E102MPD?qs=EuSGJ%252B0eAhAp2LxNcdtdzw%3D%3D</t>
+  </si>
+  <si>
+    <t>870025574003</t>
+  </si>
+  <si>
+    <t>68uf</t>
+  </si>
+  <si>
+    <t>8x8x3.5mm Rad</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/870025574003?qs=0KOYDY2FL29sdAoPfg4aVQ%3D%3D</t>
+  </si>
+  <si>
+    <t>A750KK107M1EAAE040</t>
+  </si>
+  <si>
+    <t>100uf</t>
   </si>
   <si>
     <t>CL21A226MAYNNNE</t>
   </si>
   <si>
+    <t>22uf</t>
+  </si>
+  <si>
+    <t>1210</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL32B226KAJNNNE?qs=349EhDEZ59oxUqah7LWaWw%3D%3D</t>
+  </si>
+  <si>
+    <t>CL31B106KAHNFNE</t>
+  </si>
+  <si>
     <t>10uf</t>
   </si>
   <si>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL31B106KAHNFNE?qs=xZ%2FP%252Ba9zWqbvZ%2FuLWvQDdQ%3D%3D</t>
+  </si>
+  <si>
+    <t>CL21B475KAFNNNE</t>
+  </si>
+  <si>
+    <t>4.7uf</t>
+  </si>
+  <si>
     <t>0805</t>
   </si>
   <si>
-    <t>4.7uf</t>
-  </si>
-  <si>
-    <t>Tolerance</t>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL21B475KAFNNNE?qs=fer0DVZjnG76MxvRzgkzzw%3D%3D</t>
+  </si>
+  <si>
+    <t>CL21B225KAFNNNG</t>
   </si>
   <si>
     <t>2.2uf</t>
   </si>
   <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL21B225KAFNNNG?qs=yOVawPpwOwljM4cRphaUPg%3D%3D</t>
+  </si>
+  <si>
+    <t>CL10B105KA8NFNC</t>
+  </si>
+  <si>
     <t>1uf</t>
   </si>
   <si>
-    <t>22uf</t>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL10B105KA8NFNC?qs=X6jEic%2FHinCX1Q8xescSYA%3D%3D</t>
+  </si>
+  <si>
+    <t>CL10B104KA8NNNC</t>
   </si>
   <si>
     <t>100nf</t>
   </si>
   <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL10B104KA8NNNC?qs=349EhDEZ59rmu3pGeZXx0A%3D%3D</t>
+  </si>
+  <si>
+    <t>CL10B223KB85PNC</t>
+  </si>
+  <si>
     <t>22nf</t>
   </si>
   <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL10B223KB85PNC?qs=349EhDEZ59qBh%2F6I4zsEtA%3D%3D</t>
+  </si>
+  <si>
+    <t>CL03B221KA3NNNC</t>
+  </si>
+  <si>
+    <t>220pf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL03B221KA3NNNC?qs=47mY1nHWefTe9eNIIKkdYQ%3D%3D</t>
+  </si>
+  <si>
+    <t>CL10C200JB8NNNC</t>
+  </si>
+  <si>
+    <t>20pf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL10C200JB8NNNC?qs=X6jEic%2FHinCxVzG4eDnU5g%3D%3D</t>
+  </si>
+  <si>
+    <t>SN74HC04DBRG4</t>
+  </si>
+  <si>
+    <t>SSOP-14</t>
+  </si>
+  <si>
     <t>https://www.mouser.com/ProductDetail/Texas-Instruments/SN74HC04DBRG4?qs=XQzc%252BbSrk58m%252Bx0j7t4flA%3D%3D</t>
   </si>
   <si>
-    <t>SN74HC04DBRG4</t>
-  </si>
-  <si>
-    <t>SSOP-14</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>6N137S-TA1</t>
   </si>
   <si>
@@ -128,22 +248,55 @@
     <t>https://www.mouser.com/ProductDetail/Lite-On/6N137S-TA1?qs=PByDJ0nQNwrChwHSrgNi1w%3D%3D</t>
   </si>
   <si>
+    <t>LM324DR</t>
+  </si>
+  <si>
+    <t>SOIC-14</t>
+  </si>
+  <si>
     <t>https://www.mouser.com/ProductDetail/Texas-Instruments/LM324DR?qs=KaAwwOlwaps1n%2FWkYDapEg%3D%3D</t>
   </si>
   <si>
-    <t>SOIC-14</t>
-  </si>
-  <si>
-    <t>LM324DR</t>
+    <t>INA180A1</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/INA180A1IDBVT/7219027?s=N4IgTCBcDaIJIDkCCBGAHABlXAIgIQDUAVEAXQF8g</t>
+  </si>
+  <si>
+    <t>PJA3404_R1_00001</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Panjit/PJA3404_R1_00001?qs=sPbYRqrBIVkiUO9ZInE3tw%3D%3D</t>
+  </si>
+  <si>
+    <t>FMMT495</t>
+  </si>
+  <si>
+    <t>SOT-23-3</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Diodes-Incorporated/FMMT495TA?qs=YwPsRIUVAOcuV4OIGitV8Q%3D%3D</t>
+  </si>
+  <si>
+    <t>PTS181224V075</t>
+  </si>
+  <si>
+    <t>0.29Ohm</t>
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/Bussmann-Eaton/PTS181224V075?qs=QmibqUXyDhQsWMUFkSWVRg%3D%3D</t>
   </si>
   <si>
-    <t>0.29Ohm</t>
-  </si>
-  <si>
-    <t>PTS181224V075</t>
+    <t>AP63205WU-7</t>
+  </si>
+  <si>
+    <t>TSOT-26-6</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Diodes-Incorporated/AP63205WU-7?qs=u16ybLDytRZtkj8PzdWCOw%3D%3D</t>
   </si>
   <si>
     <t>LP2950CDT-3.3RKG</t>
@@ -173,19 +326,22 @@
     <t>https://www.mouser.com/ProductDetail/STMicroelectronics/L6902D?qs=Yc96klrMi5L2iIsse6YmdQ%3D%3D</t>
   </si>
   <si>
-    <t>INA180A1</t>
-  </si>
-  <si>
-    <t>SOT-23-5</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/texas-instruments/INA180A1IDBVT/7219027?s=N4IgTCBcDaIJIDkCCBGAHABlXAIgIQDUAVEAXQF8g</t>
-  </si>
-  <si>
-    <t>PJA3404_R1_00001</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Panjit/PJA3404_R1_00001?qs=sPbYRqrBIVkiUO9ZInE3tw%3D%3D</t>
+    <t>Enclosure</t>
+  </si>
+  <si>
+    <t>https://www.jameco.com/z/SY0207-R-Jameco-Valuepro-Metal-Enclosure-2-Piece-7-5-x-9-8-x-3-2-Gloss-Black-and-Ivory_209358.html</t>
+  </si>
+  <si>
+    <t>20x4 Character Display</t>
+  </si>
+  <si>
+    <t>https://www.jameco.com/z/SIC2004A-BLWIT-Jameco-Valuepro-20x4-Character-LCD-Module-Parallel-Display-with-I2C-Module-Blue-Backlight-for-Arduino_2304015.html</t>
+  </si>
+  <si>
+    <t>USB4125-GF-A</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/GCT/USB4125-GF-A?qs=KUoIvG%2F9IlaIQ4zBJ6gLeA%3D%3D</t>
   </si>
   <si>
     <t>STM32L152RBT6A</t>
@@ -197,31 +353,25 @@
     <t>https://www.mouser.com/ProductDetail/STMicroelectronics/STM32L152RBT6A?qs=DqCdCwOw4%2F646g2lv17dkw%3D%3D</t>
   </si>
   <si>
+    <t>STM32L100C6U6A</t>
+  </si>
+  <si>
+    <t>UFQFPN-48</t>
+  </si>
+  <si>
     <t>https://www.mouser.com/ProductDetail/STMicroelectronics/STM32L100C6U6A?qs=9MuLHSklicr37J4PyR0bYg%3D%3D</t>
   </si>
   <si>
-    <t>UFQFPN-48</t>
-  </si>
-  <si>
-    <t>STM32L100C6U6A</t>
+    <t>ATS08ASM-1</t>
   </si>
   <si>
     <t>8MHz</t>
   </si>
   <si>
-    <t>20pf</t>
-  </si>
-  <si>
-    <t>220pf</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL10C200JB8NNNC?qs=X6jEic%2FHinCxVzG4eDnU5g%3D%3D</t>
-  </si>
-  <si>
-    <t>CL10C200JB8NNNC</t>
-  </si>
-  <si>
-    <t>0603</t>
+    <t>HC-49/US-SM</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/CTS-Electronic-Components/ATS08ASM-1?qs=Mr%252BgrRYddfp%2FB5O%252BMFYkdw%3D%3D</t>
   </si>
   <si>
     <t>FS24-800-C2</t>
@@ -233,9 +383,27 @@
     <t>https://www.mouser.com/ProductDetail/Triad-Magnetics/FS24-800-C2?qs=b1anAsPanWysxDNUFWmxRA%3D%3D</t>
   </si>
   <si>
+    <t>CR75NP-220KC</t>
+  </si>
+  <si>
     <t>22uh</t>
   </si>
   <si>
+    <t>Nonstandard</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sumida-america-inc/CR75NP-220KC/1059617</t>
+  </si>
+  <si>
+    <t>CDMC6D28NP-4R7MC</t>
+  </si>
+  <si>
+    <t>4.7uh</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sumida-america-inc/CDMC6D28NP-4R7MC/2620811?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALAAxwDMdIAuoQA4AuUIAymwE4CWAOwDmIAL6EwAJhmIQKSBhwFiZcAAIAsgAkAXk1YdIIAKqD%2BbAPKpNudNgCuvXOMJSqADgDschUryEJJDkFAB0XuoArdoGIOycZhbWtvZOLhIgALRSvlB8DipB5ACsTBmZENDyaFgBqsEgtJ5lYmJAA</t>
+  </si>
+  <si>
     <t>KDV06FR180ET</t>
   </si>
   <si>
@@ -245,9 +413,15 @@
     <t>https://www.mouser.com/ProductDetail/Ohmite/KDV06FR180ET?qs=l4Gc20tDgJLuG9Oc1mkpPg%3D%3D</t>
   </si>
   <si>
+    <t>KDV12FR300ET</t>
+  </si>
+  <si>
     <t>300mOhm</t>
   </si>
   <si>
+    <t>https://www.mouser.com/ProductDetail/Ohmite/KDV12FR300ET?qs=l4Gc20tDgJJqdOINs5xdYg%3D%3D</t>
+  </si>
+  <si>
     <t>SDR03EZPF1002</t>
   </si>
   <si>
@@ -257,15 +431,15 @@
     <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/SDR03EZPF1002?qs=byeeYqUIh0Mlr2mre8duxQ%3D%3D</t>
   </si>
   <si>
+    <t>ESR03EZPF5101</t>
+  </si>
+  <si>
+    <t>5.1kOhm</t>
+  </si>
+  <si>
     <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF5101?qs=493kPxzlxfITg5G1s39ZCA%3D%3D</t>
   </si>
   <si>
-    <t>5.1kOhm</t>
-  </si>
-  <si>
-    <t>ESR03EZPF5101</t>
-  </si>
-  <si>
     <t>ESR03EZPF4701</t>
   </si>
   <si>
@@ -275,256 +449,88 @@
     <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF4701?qs=493kPxzlxfL2NnaeJoZB2Q%3D%3D</t>
   </si>
   <si>
+    <t>ESR03EZPF2001</t>
+  </si>
+  <si>
+    <t>2kOhm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF2001?qs=493kPxzlxfIsacc9Eh0USA%3D%3D</t>
+  </si>
+  <si>
+    <t>ESR03EZPF1201</t>
+  </si>
+  <si>
     <t>1.2kOhm</t>
   </si>
   <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF1201?qs=493kPxzlxfIq0F4ql8poBA%3D%3D</t>
+  </si>
+  <si>
+    <t>ESR03EZPF1001</t>
+  </si>
+  <si>
+    <t>1kOhm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF1001?qs=DyUWGjl%252BcVtUAf3p1rg3iQ%3D%3D</t>
+  </si>
+  <si>
+    <t>ESR03EZPF4700</t>
+  </si>
+  <si>
+    <t>470Ohm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF4700?qs=DyUWGjl%252BcVsZQGp8SgvEfA%3D%3D</t>
+  </si>
+  <si>
     <t>ESR03EZPF1000</t>
   </si>
   <si>
     <t>100Ohm</t>
   </si>
   <si>
-    <t>1kOhm</t>
-  </si>
-  <si>
-    <t>2kOhm</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF1000?qs=493kPxzlxfJdLkJZpX4ByA%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF2001?qs=493kPxzlxfIsacc9Eh0USA%3D%3D</t>
-  </si>
-  <si>
-    <t>ESR03EZPF2001</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF1001?qs=DyUWGjl%252BcVtUAf3p1rg3iQ%3D%3D</t>
-  </si>
-  <si>
-    <t>ESR03EZPF1001</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF1201?qs=493kPxzlxfIq0F4ql8poBA%3D%3D</t>
-  </si>
-  <si>
-    <t>ESR03EZPF1201</t>
-  </si>
-  <si>
-    <t>FMMT495</t>
-  </si>
-  <si>
-    <t>SOT-23-3</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Diodes-Incorporated/FMMT495TA?qs=YwPsRIUVAOcuV4OIGitV8Q%3D%3D</t>
-  </si>
-  <si>
-    <t>Enclosure</t>
-  </si>
-  <si>
-    <t>https://www.jameco.com/z/SY0207-R-Jameco-Valuepro-Metal-Enclosure-2-Piece-7-5-x-9-8-x-3-2-Gloss-Black-and-Ivory_209358.html</t>
-  </si>
-  <si>
-    <t>20x4 Character Display</t>
-  </si>
-  <si>
-    <t>https://www.jameco.com/z/SIC2004A-BLWIT-Jameco-Valuepro-20x4-Character-LCD-Module-Parallel-Display-with-I2C-Module-Blue-Backlight-for-Arduino_2304015.html</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>4.7uh</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/sumida-america-inc/CR75NP-220KC/1059617</t>
-  </si>
-  <si>
-    <t>CR75NP-220KC</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/sumida-america-inc/CDMC6D28NP-4R7MC/2620811?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALAAxwDMdIAuoQA4AuUIAymwE4CWAOwDmIAL6EwAJhmIQKSBhwFiZcAAIAsgAkAXk1YdIIAKqD%2BbAPKpNudNgCuvXOMJSqADgDschUryEJJDkFAB0XuoArdoGIOycZhbWtvZOLhIgALRSvlB8DipB5ACsTBmZENDyaFgBqsEgtJ5lYmJAA</t>
-  </si>
-  <si>
-    <t>CDMC6D28NP-4R7MC</t>
-  </si>
-  <si>
-    <t>870025574003</t>
-  </si>
-  <si>
-    <t>68uf</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/870025574003?qs=0KOYDY2FL29sdAoPfg4aVQ%3D%3D</t>
-  </si>
-  <si>
-    <t>A750KK107M1EAAE040</t>
-  </si>
-  <si>
-    <t>8x8x3.5mm Rad</t>
-  </si>
-  <si>
-    <t>AP63205WU-7</t>
-  </si>
-  <si>
-    <t>TSOT-26-6</t>
-  </si>
-  <si>
-    <t>USB4125-GF-A</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/GCT/USB4125-GF-A?qs=KUoIvG%2F9IlaIQ4zBJ6gLeA%3D%3D</t>
-  </si>
-  <si>
-    <t>Nonstandard</t>
-  </si>
-  <si>
-    <t>CL10B104KA8NNNC</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL10B104KA8NNNC?qs=349EhDEZ59rmu3pGeZXx0A%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL10B105KA8NFNC?qs=X6jEic%2FHinCX1Q8xescSYA%3D%3D</t>
-  </si>
-  <si>
-    <t>CL10B105KA8NFNC</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL03B221KA3NNNC?qs=47mY1nHWefTe9eNIIKkdYQ%3D%3D</t>
-  </si>
-  <si>
-    <t>CL03B221KA3NNNC</t>
-  </si>
-  <si>
-    <t>CL10B223KB85PNC</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL10B223KB85PNC?qs=349EhDEZ59qBh%2F6I4zsEtA%3D%3D</t>
-  </si>
-  <si>
-    <t>100uf</t>
-  </si>
-  <si>
-    <t>UVR1E682MHD</t>
-  </si>
-  <si>
-    <t>6.8mF</t>
-  </si>
-  <si>
-    <t>18x35.5x7.5mm</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Nichicon/UVR1E682MHD?qs=sGAEpiMZZMvwFf0viD3Y3UQjCBAmXhuzNEsRvpP9m3M%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Nichicon/UVZ1E102MPD?qs=EuSGJ%252B0eAhAp2LxNcdtdzw%3D%3D</t>
-  </si>
-  <si>
-    <t>1mF</t>
-  </si>
-  <si>
-    <t>10x20x5mm</t>
-  </si>
-  <si>
-    <t>UVZ1E102MPD</t>
+    <t>ESR03EZPF22R0</t>
+  </si>
+  <si>
+    <t>22Ohm</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF22R0?qs=493kPxzlxfL2v77xEtzYQA%3D%3D</t>
+  </si>
+  <si>
+    <t>PEC11H-4015F-S0016*</t>
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/Bourns/PEC11H-4015F-S0016?qs=7MVldsJ5UazZ6nkvCEo76Q%3D%3D</t>
   </si>
   <si>
-    <t>PEC11H-4015F-S0016*</t>
-  </si>
-  <si>
     <t>TS13-1212-73-BK-260-D</t>
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/CUI-Devices/TS13-1212-73-BK-260-D?qs=t7xnP681wgVDgyvNlgHoxQ%3D%3D</t>
   </si>
   <si>
-    <t>Part(*=Similar)</t>
+    <t>150060AS75003</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/150060AS75003?qs=Li%252BoUPsLEntY15YiEuZJ2w%3D%3D</t>
+  </si>
+  <si>
+    <t>552-*</t>
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/Deltron/552-0400-GRN?qs=lj71xN7SzAIkm5eVvW23fw%3D%3D</t>
   </si>
   <si>
-    <t>552-*</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Diodes-Incorporated/AP63205WU-7?qs=u16ybLDytRZtkj8PzdWCOw%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL21B225KAFNNNG?qs=yOVawPpwOwljM4cRphaUPg%3D%3D</t>
-  </si>
-  <si>
-    <t>CL21B225KAFNNNG</t>
-  </si>
-  <si>
-    <t>CL21B475KAFNNNE</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL21B475KAFNNNE?qs=fer0DVZjnG76MxvRzgkzzw%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL31B106KAHNFNE?qs=xZ%2FP%252Ba9zWqbvZ%2FuLWvQDdQ%3D%3D</t>
-  </si>
-  <si>
-    <t>CL31B106KAHNFNE</t>
-  </si>
-  <si>
-    <t>1206</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL32B226KAJNNNE?qs=349EhDEZ59oxUqah7LWaWw%3D%3D</t>
-  </si>
-  <si>
-    <t>1210</t>
-  </si>
-  <si>
-    <t>ATS08ASM-1</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/CTS-Electronic-Components/ATS08ASM-1?qs=Mr%252BgrRYddfp%2FB5O%252BMFYkdw%3D%3D</t>
-  </si>
-  <si>
-    <t>HC-49/US-SM</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Ohmite/KDV12FR300ET?qs=l4Gc20tDgJJqdOINs5xdYg%3D%3D</t>
-  </si>
-  <si>
-    <t>KDV12FR300ET</t>
-  </si>
-  <si>
-    <t>ESR03EZPF22R0</t>
-  </si>
-  <si>
-    <t>22Ohm</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF22R0?qs=493kPxzlxfL2v77xEtzYQA%3D%3D</t>
-  </si>
-  <si>
-    <t>ESR03EZPF4700</t>
-  </si>
-  <si>
-    <t>470Ohm</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/ROHM-Semiconductor/ESR03EZPF4700?qs=DyUWGjl%252BcVsZQGp8SgvEfA%3D%3D</t>
-  </si>
-  <si>
-    <t>PMEG3020CEP,115</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Nexperia/PMEG3020CEP115?qs=LMSg3oBIm%2Fgs8Me4yQ8MUQ%3D%3D</t>
-  </si>
-  <si>
-    <t>150060AS75003</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/150060AS75003?qs=Li%252BoUPsLEntY15YiEuZJ2w%3D%3D</t>
+    <t>101-166</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/on-shore-technology-inc/101-166/2794214</t>
   </si>
   <si>
     <t>302-S161</t>
@@ -533,34 +539,31 @@
     <t>https://www.digikey.com/en/products/detail/on-shore-technology-inc/302-S161/2794234</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/on-shore-technology-inc/101-166/2794214</t>
-  </si>
-  <si>
-    <t>101-166</t>
+    <t>AWG28-16/G/300</t>
+  </si>
+  <si>
+    <t>12/300</t>
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/assmann-wsw-components/AWG28-16-G-300/655756</t>
   </si>
   <si>
-    <t>AWG28-16/G/300</t>
-  </si>
-  <si>
-    <t>12/300</t>
-  </si>
-  <si>
     <t>Front Panel PCB</t>
   </si>
   <si>
+    <t>1/1000</t>
+  </si>
+  <si>
     <t>Main PCB</t>
   </si>
   <si>
-    <t>1/1000</t>
-  </si>
-  <si>
     <t>Front Panel Laminate</t>
   </si>
   <si>
     <t>Front Panel Switch</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Carling-Technologies/LRA211-RS-B-125N?qs=etbliQ06%252B%252BUE6cQmhYT2Sw%3D%3D</t>
   </si>
   <si>
     <t>AC Power Plug</t>
@@ -576,7 +579,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -947,13 +950,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABF4B5B-D5F0-478D-961E-5722ED7FBC19}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="6" max="7" width="9.85546875" customWidth="1"/>
@@ -962,41 +965,41 @@
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
       <c r="J1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -1012,25 +1015,25 @@
         <v>1.272</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>160</v>
+        <v>14</v>
       </c>
       <c r="J2">
         <f>SUM(E:E)</f>
-        <v>100.28845200000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>99.558452000000045</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -1046,21 +1049,21 @@
         <v>0.79</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1076,21 +1079,21 @@
         <v>4.04</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>20</v>
       </c>
       <c r="G4" s="4">
         <v>0.2</v>
       </c>
       <c r="H4" t="s">
-        <v>125</v>
+        <v>21</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1106,21 +1109,21 @@
         <v>0.874</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>24</v>
       </c>
       <c r="G5" s="4">
         <v>0.2</v>
       </c>
       <c r="H5" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1136,21 +1139,21 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>28</v>
       </c>
       <c r="G6" s="4">
         <v>0.2</v>
       </c>
       <c r="H6" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1166,21 +1169,21 @@
         <v>0.36</v>
       </c>
       <c r="F7" t="s">
-        <v>122</v>
+        <v>32</v>
       </c>
       <c r="G7" s="4">
         <v>0.2</v>
       </c>
       <c r="H7" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -1196,21 +1199,21 @@
         <v>2.04</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="G8" s="4">
         <v>0.1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>147</v>
+        <v>35</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -1226,21 +1229,21 @@
         <v>0.28800000000000003</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="G9" s="4">
         <v>0.1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>145</v>
+        <v>39</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1256,21 +1259,21 @@
         <v>0.252</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="G10" s="4">
         <v>0.1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1286,21 +1289,21 @@
         <v>0.05</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="G11" s="4">
         <v>0.1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>48</v>
       </c>
       <c r="B12">
         <v>9</v>
@@ -1316,21 +1319,21 @@
         <v>9.8999999999999991E-2</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="G12" s="4">
         <v>0.1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>52</v>
       </c>
       <c r="B13">
         <v>17</v>
@@ -1346,21 +1349,21 @@
         <v>0.11900000000000001</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="G13" s="4">
         <v>0.1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1376,21 +1379,21 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="G14" s="4">
         <v>0.1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>58</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1406,21 +1409,21 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G15" s="4">
         <v>0.1</v>
       </c>
       <c r="H15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
         <v>61</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>60</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -1436,21 +1439,21 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G16" s="4">
         <v>0.05</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -1466,21 +1469,21 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1496,21 +1499,21 @@
         <v>0.56599999999999995</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -1526,21 +1529,21 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -1556,21 +1559,21 @@
         <v>0.95679999999999998</v>
       </c>
       <c r="F20" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -1586,21 +1589,21 @@
         <v>0.49199999999999999</v>
       </c>
       <c r="F21" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -1616,21 +1619,21 @@
         <v>0.248</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1646,21 +1649,21 @@
         <v>0.22800000000000001</v>
       </c>
       <c r="F23" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H23" s="2">
         <v>1812</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1676,21 +1679,21 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1706,21 +1709,21 @@
         <v>0.65600000000000003</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -1736,21 +1739,21 @@
         <v>6.82</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -1766,21 +1769,21 @@
         <v>3.92</v>
       </c>
       <c r="F27" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1796,21 +1799,21 @@
         <v>12.95</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1826,21 +1829,21 @@
         <v>10.95</v>
       </c>
       <c r="F29" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1856,21 +1859,21 @@
         <v>0.33200000000000002</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1886,21 +1889,21 @@
         <v>4.51</v>
       </c>
       <c r="F31" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1916,21 +1919,21 @@
         <v>2.95</v>
       </c>
       <c r="F32" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1946,21 +1949,21 @@
         <v>0.30599999999999999</v>
       </c>
       <c r="F33" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="G33" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H33" t="s">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1976,21 +1979,21 @@
         <v>9.82</v>
       </c>
       <c r="F34" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>63</v>
+        <v>113</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -2006,21 +2009,21 @@
         <v>0.99119999999999997</v>
       </c>
       <c r="F35" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="G35" s="4">
         <v>0.1</v>
       </c>
       <c r="H35" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -2036,21 +2039,21 @@
         <v>1.1457599999999999</v>
       </c>
       <c r="F36" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="G36" s="4">
         <v>0.2</v>
       </c>
       <c r="H36" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>122</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -2066,21 +2069,21 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="F37" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="G37" s="4">
         <v>0.01</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -2096,21 +2099,21 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="F38" t="s">
-        <v>69</v>
+        <v>126</v>
       </c>
       <c r="G38" s="4">
         <v>0.01</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>145</v>
+        <v>39</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>128</v>
       </c>
       <c r="B39">
         <v>8</v>
@@ -2126,21 +2129,21 @@
         <v>0.16800000000000001</v>
       </c>
       <c r="F39" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="G39" s="4">
         <v>0.01</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -2156,21 +2159,21 @@
         <v>0.16800000000000001</v>
       </c>
       <c r="F40" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="G40" s="4">
         <v>0.01</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -2186,21 +2189,21 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="F41" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="G41" s="4">
         <v>0.01</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="B42">
         <v>20</v>
@@ -2216,21 +2219,21 @@
         <v>0.48</v>
       </c>
       <c r="F42" t="s">
-        <v>83</v>
+        <v>138</v>
       </c>
       <c r="G42" s="4">
         <v>0.01</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="B43">
         <v>6</v>
@@ -2246,21 +2249,21 @@
         <v>0.126</v>
       </c>
       <c r="F43" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="G43" s="4">
         <v>0.01</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="B44">
         <v>32</v>
@@ -2276,21 +2279,21 @@
         <v>0.67200000000000004</v>
       </c>
       <c r="F44" t="s">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="G44" s="4">
         <v>0.01</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -2306,21 +2309,21 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="F45" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="G45" s="4">
         <v>0.01</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>149</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -2336,21 +2339,21 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F46" t="s">
-        <v>81</v>
+        <v>150</v>
       </c>
       <c r="G46" s="4">
         <v>0.01</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -2366,21 +2369,21 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="F47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G47" s="4">
         <v>0.01</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I47" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>132</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2396,21 +2399,21 @@
         <v>1.62</v>
       </c>
       <c r="F48" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G48" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H48" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="B49">
         <v>22</v>
@@ -2426,21 +2429,21 @@
         <v>3.4980000000000002</v>
       </c>
       <c r="F49" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G49" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H49" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B50">
         <v>4</v>
@@ -2456,21 +2459,21 @@
         <v>0.90400000000000003</v>
       </c>
       <c r="F50" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G50" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H50" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="B51">
         <v>5</v>
@@ -2486,21 +2489,21 @@
         <v>8.1499999999999986</v>
       </c>
       <c r="F51" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H51" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B52">
         <v>2</v>
@@ -2516,21 +2519,21 @@
         <v>0.3528</v>
       </c>
       <c r="F52" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H52" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I52" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>163</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -2546,24 +2549,24 @@
         <v>0.39322000000000001</v>
       </c>
       <c r="F53" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G53" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H53" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
+        <v>167</v>
+      </c>
+      <c r="B54" t="s">
         <v>168</v>
-      </c>
-      <c r="B54" t="s">
-        <v>169</v>
       </c>
       <c r="C54">
         <v>134.63</v>
@@ -2576,24 +2579,24 @@
         <v>3.4600720000000003</v>
       </c>
       <c r="F54" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G54" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H54" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>170</v>
       </c>
       <c r="B55" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C55">
         <v>7.3</v>
@@ -2605,21 +2608,21 @@
         <v>3.8929999999999998</v>
       </c>
       <c r="F55" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G55" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H55" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B56" t="s">
         <v>171</v>
-      </c>
-      <c r="B56" t="s">
-        <v>172</v>
       </c>
       <c r="C56">
         <v>39.9</v>
@@ -2631,16 +2634,16 @@
         <v>1.4476</v>
       </c>
       <c r="F56" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G56" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>173</v>
       </c>
@@ -2657,16 +2660,16 @@
         <v>2</v>
       </c>
       <c r="F57" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G57" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H57" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>174</v>
       </c>
@@ -2674,30 +2677,34 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>1.94</v>
       </c>
       <c r="D58">
-        <v>2</v>
+        <v>1.27</v>
       </c>
       <c r="E58">
-        <v>2</v>
+        <f>D58*B58</f>
+        <v>1.27</v>
       </c>
       <c r="F58" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G58" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H58" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C59">
         <v>1.49</v>
@@ -2709,17 +2716,20 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="F59" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G59" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="H59" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>177</v>
-      </c>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="I60" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2777,8 +2787,9 @@
     <hyperlink ref="I53" r:id="rId51" xr:uid="{EAFB691C-4ADE-428E-81AC-6D2B97C9DC3A}"/>
     <hyperlink ref="I54" r:id="rId52" xr:uid="{4DA17443-F6C2-4692-9117-EB14CD806E18}"/>
     <hyperlink ref="I59" r:id="rId53" xr:uid="{1442F385-FF75-4D4E-BC13-A9E9F1D00FE3}"/>
+    <hyperlink ref="I58" r:id="rId54" xr:uid="{FCC7A2D7-2211-4146-ADDB-2CFA25BDDA31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId54"/>
+  <pageSetup orientation="portrait" r:id="rId55"/>
 </worksheet>
 </file>
</xml_diff>